<commit_message>
Updated the back-up excel files
</commit_message>
<xml_diff>
--- a/assets/text.xlsx
+++ b/assets/text.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Kochnev\PUBLIC\securitycrisis_dashboard\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artem\Desktop\Projects\Academic\wiiw_projects\dashboarddb\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{FEC4E858-C506-4CA2-BAB2-301222E49B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE52F3B-4F91-4795-BEA0-0EB6533F28A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>paragraph</t>
   </si>
@@ -69,7 +66,64 @@
     <t>The Ukrainian economy so far has shown remarkable macro-financial resilience. However, this may change as many companies stop functioning and as unemployment rises. Banks will face substantial losses, due to the damage caused to their physical assets and the high probability of defaults on many loans. Western financial support will become ever more important as the war continues.</t>
   </si>
   <si>
-    <t>Turning to Russia, sanctions will have a very serious impact on that country’s economy and financial sector. wiiw estimate that Russian GDP will contract by at least 7-8% this year and inflation will accelerate to close to 30% by the end of 2022. During the first week of the crisis, Russia faced capital flight, FX depreciation and deposit outflows. However, the range of estimates in the economists' community is broad with some analysts predicting the GDP contraction by 15% within a year. Despite being partly hamstrung by the fact that a large proportion of Russian reserve assets are frozen in the EU and G7, the central bank managed to stabilise financial markets by a combination of confidence-building and hard-steering measures: capital controls, FX controls, regulatory easing for financial institutions, and a doubling of the key policy rate. Although these measures were effective in curtailing financial panic, they further undermined investor confidence and increased the costs of borrowing for business. The fiscal stimulus so far announced is very limited, especially considering the likely scale of the contraction, and is not going to offset a sharp decline in real household incomes in 2022.</t>
+    <t>label</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>key_damage</t>
+  </si>
+  <si>
+    <t>ukraine_costs</t>
+  </si>
+  <si>
+    <t>ukraine_macro</t>
+  </si>
+  <si>
+    <t>russia_economy</t>
+  </si>
+  <si>
+    <t>europe_inflation</t>
+  </si>
+  <si>
+    <t>europe_trade_exposure</t>
+  </si>
+  <si>
+    <t>europe_energy</t>
+  </si>
+  <si>
+    <t>europe_finance</t>
+  </si>
+  <si>
+    <t>outlook_ukraine</t>
+  </si>
+  <si>
+    <t>outlook_russia</t>
+  </si>
+  <si>
+    <t>outlook_eu</t>
+  </si>
+  <si>
+    <t>russia_policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turning to Russia, sanctions will have a very serious impact on that country’s economy and financial sector. wiiw estimate that Russian GDP will contract by at least 7-8% this year and inflation will accelerate to close to 30% by the end of 2022. During the first week of the crisis, Russia faced capital flight, FX depreciation and deposit outflows. However, the range of estimates in the economists' community is broad with some analysts predicting the GDP contraction by 15% within a year. </t>
+  </si>
+  <si>
+    <t>Despite being partly hamstrung by the fact that a large proportion of Russian reserve assets are frozen in the EU and G7, the central bank managed to stabilise financial markets by a combination of confidence-building and hard-steering measures: capital controls, FX controls, regulatory easing for financial institutions, and a doubling of the key policy rate. Although these measures were effective in curtailing financial panic, they further undermined investor confidence and increased the costs of borrowing for business. The fiscal stimulus so far announced is very limited, especially considering the likely scale of the contraction, and is not going to offset a sharp decline in real household incomes in 2022.</t>
+  </si>
+  <si>
+    <t>europe_refugees</t>
+  </si>
+  <si>
+    <t>policies</t>
+  </si>
+  <si>
+    <t>russia_sanctions</t>
+  </si>
+  <si>
+    <t>There are several caveats surrounding the sanctions' impact. First, quantity is not quality. Most of the sanctions impose restrictions on individuals and have a limited impact on the aggregate economy. Most importantly, the EU has still not imposed an energy embargo, which would have the biggest impact on the Russian fiscal position. Second, it is impossible to effectively impose sanctions exclusively against elites, without harming the general population. Sector-wide sanctions will cause hardship for ordinary Russians, but even individual-related sanctions do not avoid collateral damage. Evidence from Russia and other countries suggests that governments are likely to compensate the elites for their losses at the expense of taxpayers. There is a high chance that campaigns to boycott all Russian public institutions, together with the exodus of Western franchises from the Russian market, will affect mainly well-educated Russians living in big cities – those very people who value individuality over grand political achievements, who deliver and consume diverse media content, and who are most critical of the Putin regime. With their income opportunities and information flows constrained, they will become more dependent on state-provided revenues. This, in turn, will increase the likelihood that they are co-opted and that the anti-Western sentiment in Russia will harden.</t>
   </si>
 </sst>
 </file>
@@ -123,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -135,6 +189,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -441,138 +501,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" style="1"/>
+    <col min="1" max="1" width="24.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="119.75" style="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="10" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    </row>
+    <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    </row>
+    <row r="12" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    </row>
+    <row r="13" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    </row>
+    <row r="14" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    </row>
+    <row r="15" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    </row>
+    <row r="16" spans="1:2" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="17" spans="1:2" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>